<commit_message>
second version with A stocks
</commit_message>
<xml_diff>
--- a/汽车-ST亚星历史数据.xlsx
+++ b/汽车-ST亚星历史数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/PycharmProjects/train/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA54310-597C-D042-8C51-A83877C8A2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64F3DE-3C3C-3B4F-9EE9-18D28589F7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="1540" windowWidth="16100" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST亚星资产负债表" sheetId="1" r:id="rId1"/>
@@ -20,68 +20,12 @@
     <sheet name="成本收入比率" sheetId="5" r:id="rId5"/>
     <sheet name="其他指标-年报" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">成本收入比率!$B$14:$F$14</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">成本收入比率!$B$15:$F$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">成本收入比率!$B$10:$F$10</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">成本收入比率!$B$11:$F$11</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">成本收入比率!$B$12:$F$12</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">成本收入比率!$B$13:$F$13</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="1076">
   <si>
     <t>科目\年度</t>
   </si>
@@ -893,10 +837,10 @@
     <t>147700.00</t>
   </si>
   <si>
-    <t>97900.00</t>
-  </si>
-  <si>
-    <t>187900.00</t>
+    <t>95000.00</t>
+  </si>
+  <si>
+    <t>185000.00</t>
   </si>
   <si>
     <t>270800.00</t>
@@ -935,10 +879,10 @@
     <t>161700.00</t>
   </si>
   <si>
-    <t>116800.00</t>
-  </si>
-  <si>
-    <t>208000.00</t>
+    <t>113900.00</t>
+  </si>
+  <si>
+    <t>205100.00</t>
   </si>
   <si>
     <t>268600.00</t>
@@ -1058,10 +1002,10 @@
     <t>135100.00</t>
   </si>
   <si>
-    <t>91600.00</t>
-  </si>
-  <si>
-    <t>170200.00</t>
+    <t>88800.00</t>
+  </si>
+  <si>
+    <t>167300.00</t>
   </si>
   <si>
     <t>223300.00</t>
@@ -1970,10 +1914,7 @@
     <t>172900.00</t>
   </si>
   <si>
-    <t>166300.00</t>
-  </si>
-  <si>
-    <t>251100.00</t>
+    <t>248600.00</t>
   </si>
   <si>
     <t>250600.00</t>
@@ -2090,18 +2031,15 @@
     <t>177300.00</t>
   </si>
   <si>
-    <t>186000.00</t>
-  </si>
-  <si>
-    <t>256100.00</t>
+    <t>183200.00</t>
+  </si>
+  <si>
+    <t>253600.00</t>
   </si>
   <si>
     <t>260300.00</t>
   </si>
   <si>
-    <t>185000.00</t>
-  </si>
-  <si>
     <t>141800.00</t>
   </si>
   <si>
@@ -2129,10 +2067,10 @@
     <t>104600.00</t>
   </si>
   <si>
-    <t>89000.00</t>
-  </si>
-  <si>
-    <t>184200.00</t>
+    <t>86100.00</t>
+  </si>
+  <si>
+    <t>181700.00</t>
   </si>
   <si>
     <t>209500.00</t>
@@ -2270,10 +2208,10 @@
     <t>148100.00</t>
   </si>
   <si>
-    <t>123500.00</t>
-  </si>
-  <si>
-    <t>214700.00</t>
+    <t>120700.00</t>
+  </si>
+  <si>
+    <t>212200.00</t>
   </si>
   <si>
     <t>248900.00</t>
@@ -3322,7 +3260,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -3335,8 +3273,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3398,10 +3338,10 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3506,10 +3446,10 @@
                   <c:v>1.09478672985782</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1930541368743619</c:v>
+                  <c:v>1.198947368421053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.106971793507185</c:v>
+                  <c:v>1.1086486486486491</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.99187592319054652</c:v>
@@ -3519,7 +3459,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CDAC-C947-BD74-5B633CC46662}"/>
+              <c16:uniqueId val="{00000000-AA7E-4F45-845F-DB7144CF9D9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3571,10 +3511,10 @@
                   <c:v>7.9214624238320916E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0922880490296223E-2</c:v>
+                  <c:v>8.339315789473685E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2694890899414593E-2</c:v>
+                  <c:v>5.3520918918918921E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.0221565731166908E-2</c:v>
@@ -3584,7 +3524,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CDAC-C947-BD74-5B633CC46662}"/>
+              <c16:uniqueId val="{00000001-AA7E-4F45-845F-DB7144CF9D9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3636,10 +3576,10 @@
                   <c:v>2.711726472579553E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0201225740551579E-2</c:v>
+                  <c:v>4.142842105263158E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1448110697179348E-2</c:v>
+                  <c:v>2.1784324324324329E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.723456425406204E-2</c:v>
@@ -3649,7 +3589,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CDAC-C947-BD74-5B633CC46662}"/>
+              <c16:uniqueId val="{00000002-AA7E-4F45-845F-DB7144CF9D9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3701,10 +3641,10 @@
                   <c:v>5.1223290453622207E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7378855975485194E-2</c:v>
+                  <c:v>6.9435684210526316E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1411814795103778E-2</c:v>
+                  <c:v>3.1904216216216218E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.2807680945347119E-2</c:v>
@@ -3714,7 +3654,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-CDAC-C947-BD74-5B633CC46662}"/>
+              <c16:uniqueId val="{00000003-AA7E-4F45-845F-DB7144CF9D9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3766,10 +3706,10 @@
                   <c:v>-0.25420399458361542</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.38328988764044952</c:v>
+                  <c:v>-0.39499031578947369</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.21335838211814789</c:v>
+                  <c:v>-0.21670291891891891</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-9.2775480059084189E-2</c:v>
@@ -3779,7 +3719,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-CDAC-C947-BD74-5B633CC46662}"/>
+              <c16:uniqueId val="{00000004-AA7E-4F45-845F-DB7144CF9D9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4168,7 +4108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4537,19 +4477,19 @@
         <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -5553,7 +5493,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7546,7 +7486,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7968,204 +7908,204 @@
         <v>628</v>
       </c>
       <c r="E10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10" t="s">
         <v>629</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>630</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>631</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>632</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>633</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>634</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>635</v>
-      </c>
-      <c r="L10" t="s">
-        <v>636</v>
       </c>
       <c r="M10" t="s">
         <v>132</v>
       </c>
       <c r="N10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>637</v>
+      </c>
+      <c r="B11" t="s">
         <v>638</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>639</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>640</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>641</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>642</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>643</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>644</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>645</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>646</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>647</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>648</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>649</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>650</v>
-      </c>
-      <c r="N11" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>651</v>
+      </c>
+      <c r="B12" t="s">
         <v>652</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>653</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>654</v>
-      </c>
-      <c r="D12" t="s">
-        <v>655</v>
       </c>
       <c r="E12" t="s">
         <v>618</v>
       </c>
       <c r="F12" t="s">
+        <v>655</v>
+      </c>
+      <c r="G12" t="s">
         <v>656</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>657</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>658</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>659</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>660</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>661</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>662</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>663</v>
-      </c>
-      <c r="N12" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>664</v>
+      </c>
+      <c r="B13" t="s">
         <v>665</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>666</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>667</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>668</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>669</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>670</v>
-      </c>
-      <c r="G13" t="s">
-        <v>671</v>
       </c>
       <c r="H13" t="s">
         <v>628</v>
       </c>
       <c r="I13" t="s">
+        <v>271</v>
+      </c>
+      <c r="J13" t="s">
+        <v>671</v>
+      </c>
+      <c r="K13" t="s">
         <v>672</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>673</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>674</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>675</v>
-      </c>
-      <c r="M13" t="s">
-        <v>676</v>
-      </c>
-      <c r="N13" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>676</v>
+      </c>
+      <c r="B14" t="s">
+        <v>677</v>
+      </c>
+      <c r="C14" t="s">
         <v>678</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>679</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>680</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>681</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>682</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>683</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>684</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>685</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>686</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>687</v>
-      </c>
-      <c r="K14" t="s">
-        <v>688</v>
-      </c>
-      <c r="L14" t="s">
-        <v>689</v>
       </c>
       <c r="M14" t="s">
         <v>129</v>
@@ -8176,25 +8116,25 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>688</v>
+      </c>
+      <c r="B15" t="s">
+        <v>689</v>
+      </c>
+      <c r="C15" t="s">
         <v>690</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>691</v>
-      </c>
-      <c r="C15" t="s">
-        <v>692</v>
-      </c>
-      <c r="D15" t="s">
-        <v>693</v>
       </c>
       <c r="E15" t="s">
         <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G15" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H15" t="s">
         <v>167</v>
@@ -8203,156 +8143,156 @@
         <v>351</v>
       </c>
       <c r="J15" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="K15" t="s">
         <v>86</v>
       </c>
       <c r="L15" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="M15" t="s">
         <v>571</v>
       </c>
       <c r="N15" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>697</v>
+      </c>
+      <c r="B16" t="s">
+        <v>698</v>
+      </c>
+      <c r="C16" t="s">
         <v>699</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>700</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>701</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>702</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>703</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>704</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>705</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>706</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>707</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>708</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>709</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>710</v>
-      </c>
-      <c r="M16" t="s">
-        <v>711</v>
-      </c>
-      <c r="N16" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>711</v>
+      </c>
+      <c r="B17" t="s">
+        <v>712</v>
+      </c>
+      <c r="C17" t="s">
         <v>713</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>714</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>715</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>716</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>717</v>
-      </c>
-      <c r="F17" t="s">
-        <v>718</v>
-      </c>
-      <c r="G17" t="s">
-        <v>719</v>
       </c>
       <c r="H17" t="s">
         <v>356</v>
       </c>
       <c r="I17" t="s">
+        <v>718</v>
+      </c>
+      <c r="J17" t="s">
+        <v>719</v>
+      </c>
+      <c r="K17" t="s">
         <v>720</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>721</v>
-      </c>
-      <c r="K17" t="s">
-        <v>722</v>
-      </c>
-      <c r="L17" t="s">
-        <v>723</v>
       </c>
       <c r="M17" t="s">
         <v>392</v>
       </c>
       <c r="N17" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>723</v>
+      </c>
+      <c r="B18" t="s">
+        <v>724</v>
+      </c>
+      <c r="C18" t="s">
         <v>725</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>726</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>727</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>728</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>729</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>730</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>731</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
+        <v>730</v>
+      </c>
+      <c r="K18" t="s">
         <v>732</v>
       </c>
-      <c r="I18" t="s">
+      <c r="L18" t="s">
         <v>733</v>
       </c>
-      <c r="J18" t="s">
-        <v>732</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>734</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>735</v>
-      </c>
-      <c r="M18" t="s">
-        <v>736</v>
-      </c>
-      <c r="N18" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B19" t="s">
         <v>573</v>
@@ -8396,7 +8336,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -8440,7 +8380,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -8461,7 +8401,7 @@
         <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I21" t="s">
         <v>7</v>
@@ -8484,7 +8424,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -8505,7 +8445,7 @@
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I22" t="s">
         <v>441</v>
@@ -8528,51 +8468,51 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>742</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>743</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
         <v>744</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="I23" t="s">
         <v>745</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" t="s">
         <v>746</v>
       </c>
-      <c r="I23" t="s">
+      <c r="L23" t="s">
         <v>747</v>
       </c>
-      <c r="J23" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>748</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>749</v>
-      </c>
-      <c r="M23" t="s">
-        <v>750</v>
-      </c>
-      <c r="N23" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -8608,7 +8548,7 @@
         <v>7</v>
       </c>
       <c r="M24" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N24" t="s">
         <v>7</v>
@@ -8616,95 +8556,95 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>752</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>743</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>753</v>
+      </c>
+      <c r="I25" t="s">
         <v>754</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>745</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" t="s">
-        <v>755</v>
-      </c>
-      <c r="I25" t="s">
-        <v>756</v>
       </c>
       <c r="J25" t="s">
         <v>442</v>
       </c>
       <c r="K25" t="s">
+        <v>755</v>
+      </c>
+      <c r="L25" t="s">
+        <v>756</v>
+      </c>
+      <c r="M25" t="s">
         <v>757</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>758</v>
-      </c>
-      <c r="M25" t="s">
-        <v>759</v>
-      </c>
-      <c r="N25" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>759</v>
+      </c>
+      <c r="B26" t="s">
+        <v>760</v>
+      </c>
+      <c r="C26" t="s">
         <v>761</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>762</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>763</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>764</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>765</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>766</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>767</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>768</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>769</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>770</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>771</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>772</v>
-      </c>
-      <c r="M26" t="s">
-        <v>773</v>
-      </c>
-      <c r="N26" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -8748,7 +8688,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -8769,7 +8709,7 @@
         <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="I28" t="s">
         <v>7</v>
@@ -8792,51 +8732,51 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B29" t="s">
+        <v>760</v>
+      </c>
+      <c r="C29" t="s">
+        <v>761</v>
+      </c>
+      <c r="D29" t="s">
         <v>762</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>763</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>764</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>765</v>
       </c>
-      <c r="F29" t="s">
-        <v>766</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
+        <v>777</v>
+      </c>
+      <c r="I29" t="s">
         <v>767</v>
       </c>
-      <c r="H29" t="s">
-        <v>779</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
+        <v>768</v>
+      </c>
+      <c r="K29" t="s">
         <v>769</v>
       </c>
-      <c r="J29" t="s">
+      <c r="L29" t="s">
         <v>770</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>771</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>772</v>
-      </c>
-      <c r="M29" t="s">
-        <v>773</v>
-      </c>
-      <c r="N29" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B30" t="s">
         <v>587</v>
@@ -8880,7 +8820,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -8924,7 +8864,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -8933,7 +8873,7 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -8968,51 +8908,51 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>782</v>
+      </c>
+      <c r="B33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C33" t="s">
         <v>784</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>785</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>786</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>787</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>788</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>789</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>790</v>
-      </c>
-      <c r="H33" t="s">
-        <v>791</v>
-      </c>
-      <c r="I33" t="s">
-        <v>792</v>
       </c>
       <c r="J33" t="s">
         <v>181</v>
       </c>
       <c r="K33" t="s">
+        <v>791</v>
+      </c>
+      <c r="L33" t="s">
+        <v>792</v>
+      </c>
+      <c r="M33" t="s">
         <v>793</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>794</v>
-      </c>
-      <c r="M33" t="s">
-        <v>795</v>
-      </c>
-      <c r="N33" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -9056,87 +8996,87 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B35" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C35" t="s">
+        <v>784</v>
+      </c>
+      <c r="D35" t="s">
+        <v>797</v>
+      </c>
+      <c r="E35" t="s">
         <v>786</v>
       </c>
-      <c r="D35" t="s">
-        <v>799</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
+        <v>787</v>
+      </c>
+      <c r="G35" t="s">
         <v>788</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
         <v>789</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>790</v>
-      </c>
-      <c r="H35" t="s">
-        <v>791</v>
-      </c>
-      <c r="I35" t="s">
-        <v>792</v>
       </c>
       <c r="J35" t="s">
         <v>181</v>
       </c>
       <c r="K35" t="s">
+        <v>791</v>
+      </c>
+      <c r="L35" t="s">
+        <v>792</v>
+      </c>
+      <c r="M35" t="s">
         <v>793</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>794</v>
-      </c>
-      <c r="M35" t="s">
-        <v>795</v>
-      </c>
-      <c r="N35" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B36" t="s">
         <v>117</v>
       </c>
       <c r="C36" t="s">
+        <v>799</v>
+      </c>
+      <c r="D36" t="s">
+        <v>800</v>
+      </c>
+      <c r="E36" t="s">
         <v>801</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>802</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>803</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H36" t="s">
         <v>804</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>805</v>
       </c>
-      <c r="H36" t="s">
+      <c r="J36" t="s">
         <v>806</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>807</v>
       </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
         <v>808</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>809</v>
-      </c>
-      <c r="L36" t="s">
-        <v>810</v>
-      </c>
-      <c r="M36" t="s">
-        <v>811</v>
       </c>
       <c r="N36" t="s">
         <v>352</v>
@@ -9144,22 +9084,22 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>810</v>
+      </c>
+      <c r="B37" t="s">
+        <v>811</v>
+      </c>
+      <c r="C37" t="s">
         <v>812</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>813</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>814</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F37" t="s">
         <v>815</v>
-      </c>
-      <c r="E37" t="s">
-        <v>816</v>
-      </c>
-      <c r="F37" t="s">
-        <v>817</v>
       </c>
       <c r="G37" t="s">
         <v>406</v>
@@ -9168,63 +9108,63 @@
         <v>407</v>
       </c>
       <c r="I37" t="s">
+        <v>816</v>
+      </c>
+      <c r="J37" t="s">
+        <v>817</v>
+      </c>
+      <c r="K37" t="s">
         <v>818</v>
       </c>
-      <c r="J37" t="s">
+      <c r="L37" t="s">
         <v>819</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>820</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>821</v>
-      </c>
-      <c r="M37" t="s">
-        <v>822</v>
-      </c>
-      <c r="N37" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>822</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>823</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" t="s">
         <v>824</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="M38" t="s">
         <v>825</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" t="s">
-        <v>7</v>
-      </c>
-      <c r="L38" t="s">
-        <v>826</v>
-      </c>
-      <c r="M38" t="s">
-        <v>827</v>
       </c>
       <c r="N38" t="s">
         <v>7</v>
@@ -9232,51 +9172,51 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>826</v>
+      </c>
+      <c r="B39" t="s">
+        <v>827</v>
+      </c>
+      <c r="C39" t="s">
         <v>828</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>829</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>830</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>831</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>832</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" t="s">
         <v>833</v>
       </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>834</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
         <v>835</v>
       </c>
-      <c r="I39" t="s">
+      <c r="K39" t="s">
         <v>836</v>
       </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
         <v>837</v>
       </c>
-      <c r="K39" t="s">
+      <c r="M39" t="s">
         <v>838</v>
       </c>
-      <c r="L39" t="s">
+      <c r="N39" t="s">
         <v>839</v>
-      </c>
-      <c r="M39" t="s">
-        <v>840</v>
-      </c>
-      <c r="N39" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B40" t="s">
         <v>601</v>
@@ -9320,51 +9260,51 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>841</v>
+      </c>
+      <c r="B41" t="s">
+        <v>842</v>
+      </c>
+      <c r="C41" t="s">
         <v>843</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>844</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>845</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
         <v>846</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>847</v>
       </c>
-      <c r="F41" t="s">
+      <c r="H41" t="s">
         <v>848</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>849</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>850</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>851</v>
       </c>
-      <c r="J41" t="s">
+      <c r="L41" t="s">
         <v>852</v>
       </c>
-      <c r="K41" t="s">
+      <c r="M41" t="s">
         <v>853</v>
       </c>
-      <c r="L41" t="s">
+      <c r="N41" t="s">
         <v>854</v>
-      </c>
-      <c r="M41" t="s">
-        <v>855</v>
-      </c>
-      <c r="N41" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B42" t="s">
         <v>559</v>
@@ -9408,7 +9348,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B43" t="s">
         <v>615</v>
@@ -9447,12 +9387,12 @@
         <v>623</v>
       </c>
       <c r="N43" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B44" t="s">
         <v>614</v>
@@ -9496,7 +9436,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -9540,7 +9480,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -9584,7 +9524,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -9628,7 +9568,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -9661,7 +9601,7 @@
         <v>427</v>
       </c>
       <c r="L48" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="M48" t="s">
         <v>429</v>
@@ -9672,213 +9612,213 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>864</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>865</v>
+      </c>
+      <c r="D49" t="s">
         <v>866</v>
       </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>867</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F49" t="s">
         <v>868</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>869</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>870</v>
       </c>
-      <c r="G49" t="s">
+      <c r="I49" t="s">
         <v>871</v>
       </c>
-      <c r="H49" t="s">
+      <c r="J49" t="s">
         <v>872</v>
       </c>
-      <c r="I49" t="s">
+      <c r="K49" t="s">
         <v>873</v>
       </c>
-      <c r="J49" t="s">
+      <c r="L49" t="s">
         <v>874</v>
       </c>
-      <c r="K49" t="s">
+      <c r="M49" t="s">
         <v>875</v>
       </c>
-      <c r="L49" t="s">
+      <c r="N49" t="s">
         <v>876</v>
-      </c>
-      <c r="M49" t="s">
-        <v>877</v>
-      </c>
-      <c r="N49" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>877</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>878</v>
+      </c>
+      <c r="D50" t="s">
         <v>879</v>
       </c>
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>880</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>881</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>882</v>
       </c>
-      <c r="F50" t="s">
+      <c r="H50" t="s">
         <v>883</v>
       </c>
-      <c r="G50" t="s">
+      <c r="I50" t="s">
         <v>884</v>
       </c>
-      <c r="H50" t="s">
+      <c r="J50" t="s">
         <v>885</v>
       </c>
-      <c r="I50" t="s">
+      <c r="K50" t="s">
         <v>886</v>
       </c>
-      <c r="J50" t="s">
+      <c r="L50" t="s">
         <v>887</v>
       </c>
-      <c r="K50" t="s">
+      <c r="M50" t="s">
         <v>888</v>
       </c>
-      <c r="L50" t="s">
+      <c r="N50" t="s">
         <v>889</v>
-      </c>
-      <c r="M50" t="s">
-        <v>890</v>
-      </c>
-      <c r="N50" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>890</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>891</v>
+      </c>
+      <c r="D51" t="s">
         <v>892</v>
       </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>893</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>894</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>895</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
         <v>896</v>
       </c>
-      <c r="G51" t="s">
+      <c r="I51" t="s">
         <v>897</v>
       </c>
-      <c r="H51" t="s">
+      <c r="J51" t="s">
         <v>898</v>
       </c>
-      <c r="I51" t="s">
+      <c r="K51" t="s">
         <v>899</v>
       </c>
-      <c r="J51" t="s">
+      <c r="L51" t="s">
         <v>900</v>
       </c>
-      <c r="K51" t="s">
+      <c r="M51" t="s">
         <v>901</v>
       </c>
-      <c r="L51" t="s">
+      <c r="N51" t="s">
         <v>902</v>
-      </c>
-      <c r="M51" t="s">
-        <v>903</v>
-      </c>
-      <c r="N51" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>903</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>904</v>
+      </c>
+      <c r="D52" t="s">
         <v>905</v>
       </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>906</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>907</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>908</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>909</v>
       </c>
-      <c r="G52" t="s">
+      <c r="I52" t="s">
         <v>910</v>
-      </c>
-      <c r="H52" t="s">
-        <v>911</v>
-      </c>
-      <c r="I52" t="s">
-        <v>912</v>
       </c>
       <c r="J52" t="s">
         <v>524</v>
       </c>
       <c r="K52" t="s">
+        <v>911</v>
+      </c>
+      <c r="L52" t="s">
+        <v>912</v>
+      </c>
+      <c r="M52" t="s">
         <v>913</v>
       </c>
-      <c r="L52" t="s">
+      <c r="N52" t="s">
         <v>914</v>
-      </c>
-      <c r="M52" t="s">
-        <v>915</v>
-      </c>
-      <c r="N52" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>915</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>916</v>
+      </c>
+      <c r="D53" t="s">
         <v>917</v>
       </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>918</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
         <v>919</v>
       </c>
-      <c r="E53" t="s">
+      <c r="H53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53" t="s">
         <v>920</v>
-      </c>
-      <c r="F53" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" t="s">
-        <v>921</v>
-      </c>
-      <c r="H53" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" t="s">
-        <v>7</v>
-      </c>
-      <c r="J53" t="s">
-        <v>7</v>
-      </c>
-      <c r="K53" t="s">
-        <v>922</v>
       </c>
       <c r="L53" t="s">
         <v>7</v>
@@ -9892,7 +9832,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -9942,7 +9882,7 @@
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D55" t="s">
         <v>403</v>
@@ -9963,156 +9903,156 @@
         <v>408</v>
       </c>
       <c r="J55" t="s">
+        <v>923</v>
+      </c>
+      <c r="K55" t="s">
+        <v>924</v>
+      </c>
+      <c r="L55" t="s">
         <v>925</v>
       </c>
-      <c r="K55" t="s">
+      <c r="M55" t="s">
         <v>926</v>
       </c>
-      <c r="L55" t="s">
+      <c r="N55" t="s">
         <v>927</v>
-      </c>
-      <c r="M55" t="s">
-        <v>928</v>
-      </c>
-      <c r="N55" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>928</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" t="s">
+        <v>929</v>
+      </c>
+      <c r="I56" t="s">
         <v>930</v>
       </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G56" t="s">
-        <v>7</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
         <v>931</v>
       </c>
-      <c r="I56" t="s">
-        <v>932</v>
-      </c>
-      <c r="J56" t="s">
-        <v>933</v>
-      </c>
       <c r="K56" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="L56" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="M56" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="N56" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>932</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>933</v>
+      </c>
+      <c r="D57" t="s">
         <v>934</v>
       </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>935</v>
       </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
         <v>936</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>937</v>
       </c>
-      <c r="F57" t="s">
+      <c r="H57" t="s">
         <v>938</v>
       </c>
-      <c r="G57" t="s">
+      <c r="I57" t="s">
         <v>939</v>
       </c>
-      <c r="H57" t="s">
+      <c r="J57" t="s">
         <v>940</v>
       </c>
-      <c r="I57" t="s">
+      <c r="K57" t="s">
         <v>941</v>
       </c>
-      <c r="J57" t="s">
+      <c r="L57" t="s">
         <v>942</v>
       </c>
-      <c r="K57" t="s">
+      <c r="M57" t="s">
         <v>943</v>
       </c>
-      <c r="L57" t="s">
+      <c r="N57" t="s">
         <v>944</v>
-      </c>
-      <c r="M57" t="s">
-        <v>945</v>
-      </c>
-      <c r="N57" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
       </c>
       <c r="E58" t="s">
+        <v>947</v>
+      </c>
+      <c r="F58" t="s">
+        <v>948</v>
+      </c>
+      <c r="G58" t="s">
         <v>949</v>
       </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
         <v>950</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58" t="s">
         <v>951</v>
       </c>
-      <c r="H58" t="s">
+      <c r="J58" t="s">
         <v>952</v>
       </c>
-      <c r="I58" t="s">
+      <c r="K58" t="s">
         <v>953</v>
       </c>
-      <c r="J58" t="s">
+      <c r="L58" t="s">
         <v>954</v>
-      </c>
-      <c r="K58" t="s">
-        <v>955</v>
-      </c>
-      <c r="L58" t="s">
-        <v>956</v>
       </c>
       <c r="M58" t="s">
         <v>309</v>
       </c>
       <c r="N58" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -10121,25 +10061,25 @@
         <v>623</v>
       </c>
       <c r="D59" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E59" t="s">
         <v>579</v>
       </c>
       <c r="F59" t="s">
+        <v>958</v>
+      </c>
+      <c r="G59" t="s">
+        <v>959</v>
+      </c>
+      <c r="H59" t="s">
         <v>960</v>
       </c>
-      <c r="G59" t="s">
+      <c r="I59" t="s">
         <v>961</v>
       </c>
-      <c r="H59" t="s">
+      <c r="J59" t="s">
         <v>962</v>
-      </c>
-      <c r="I59" t="s">
-        <v>963</v>
-      </c>
-      <c r="J59" t="s">
-        <v>964</v>
       </c>
       <c r="K59" t="s">
         <v>356</v>
@@ -10148,59 +10088,59 @@
         <v>623</v>
       </c>
       <c r="M59" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="N59" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>965</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>966</v>
+      </c>
+      <c r="D60" t="s">
         <v>967</v>
       </c>
-      <c r="B60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>968</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>969</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>970</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>971</v>
       </c>
-      <c r="G60" t="s">
+      <c r="I60" t="s">
         <v>972</v>
       </c>
-      <c r="H60" t="s">
+      <c r="J60" t="s">
         <v>973</v>
       </c>
-      <c r="I60" t="s">
+      <c r="K60" t="s">
         <v>974</v>
       </c>
-      <c r="J60" t="s">
+      <c r="L60" t="s">
         <v>975</v>
       </c>
-      <c r="K60" t="s">
+      <c r="M60" t="s">
         <v>976</v>
       </c>
-      <c r="L60" t="s">
+      <c r="N60" t="s">
         <v>977</v>
-      </c>
-      <c r="M60" t="s">
-        <v>978</v>
-      </c>
-      <c r="N60" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -10244,7 +10184,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -10288,7 +10228,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -10332,7 +10272,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -10376,7 +10316,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -10415,12 +10355,12 @@
         <v>623</v>
       </c>
       <c r="N65" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
@@ -10463,7 +10403,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10480,25 +10420,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>986</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" t="s">
         <v>990</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>991</v>
-      </c>
-      <c r="G1" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -10518,7 +10458,7 @@
         <v>1.2633856138453221</v>
       </c>
       <c r="G2" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -10538,7 +10478,7 @@
         <v>1.2128177393185511</v>
       </c>
       <c r="G3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -10558,47 +10498,47 @@
         <v>0.94704931285367822</v>
       </c>
       <c r="G4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G5" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -10615,10 +10555,10 @@
         <v>0.40458015267175568</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G7" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -10635,30 +10575,30 @@
         <v>-0.59541984732824427</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G8" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -10669,16 +10609,16 @@
         <v>8.5308056872037921E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>6.4351378958120528E-2</v>
+        <v>6.5263157894736842E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>9.4199042043640241E-2</v>
+        <v>9.567567567567567E-2</v>
       </c>
       <c r="F10" s="3">
         <v>0.1754062038404727</v>
       </c>
       <c r="G10" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -10689,16 +10629,16 @@
         <v>-0.13067027758970889</v>
       </c>
       <c r="D11" s="3">
-        <v>-1.7644637385086821E-2</v>
+        <v>-1.8183263157894741E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>-8.3555082490686536E-2</v>
+        <v>-8.4864864864864858E-2</v>
       </c>
       <c r="F11" s="3">
         <v>5.2483382570162494E-3</v>
       </c>
       <c r="G11" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -10709,16 +10649,16 @@
         <v>0.91469194312796209</v>
       </c>
       <c r="D12" s="3">
-        <v>0.93564862104187951</v>
+        <v>0.9347368421052632</v>
       </c>
       <c r="E12" s="3">
-        <v>0.90580095795635973</v>
+        <v>0.9043243243243243</v>
       </c>
       <c r="F12" s="3">
         <v>0.82459379615952733</v>
       </c>
       <c r="G12" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -10729,16 +10669,16 @@
         <v>1.862085308056872E-3</v>
       </c>
       <c r="D13" s="3">
-        <v>1.7327885597548519E-3</v>
+        <v>1.7856842105263161E-3</v>
       </c>
       <c r="E13" s="3">
-        <v>8.3177221926556679E-4</v>
+        <v>8.4481081081081073E-4</v>
       </c>
       <c r="F13" s="3">
         <v>6.3574593796159528E-4</v>
       </c>
       <c r="G13" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -10755,10 +10695,10 @@
         <v>-3.4452490673688829E-2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G14" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -10775,10 +10715,10 @@
         <v>-0.85326086956521741</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G15" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -10789,16 +10729,16 @@
         <v>7.9214624238320916E-2</v>
       </c>
       <c r="D16" s="3">
-        <v>8.0922880490296223E-2</v>
+        <v>8.339315789473685E-2</v>
       </c>
       <c r="E16" s="3">
-        <v>5.2694890899414593E-2</v>
+        <v>5.3520918918918921E-2</v>
       </c>
       <c r="F16" s="3">
         <v>5.0221565731166908E-2</v>
       </c>
       <c r="G16" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -10809,16 +10749,16 @@
         <v>2.711726472579553E-2</v>
       </c>
       <c r="D17" s="3">
-        <v>4.0201225740551579E-2</v>
+        <v>4.142842105263158E-2</v>
       </c>
       <c r="E17" s="3">
-        <v>2.1448110697179348E-2</v>
+        <v>2.1784324324324329E-2</v>
       </c>
       <c r="F17" s="3">
         <v>1.723456425406204E-2</v>
       </c>
       <c r="G17" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -10829,16 +10769,16 @@
         <v>5.1223290453622207E-2</v>
       </c>
       <c r="D18" s="3">
-        <v>6.7378855975485194E-2</v>
+        <v>6.9435684210526316E-2</v>
       </c>
       <c r="E18" s="3">
-        <v>3.1411814795103778E-2</v>
+        <v>3.1904216216216218E-2</v>
       </c>
       <c r="F18" s="3">
         <v>3.2807680945347119E-2</v>
       </c>
       <c r="G18" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -10849,16 +10789,16 @@
         <v>1.298571428571429E-2</v>
       </c>
       <c r="D19" s="3">
-        <v>7.7552502553626154E-2</v>
+        <v>7.9919894736842106E-2</v>
       </c>
       <c r="E19" s="3">
-        <v>8.4619478445981902E-2</v>
+        <v>8.5945945945945942E-2</v>
       </c>
       <c r="F19" s="3">
         <v>3.8774002954209748E-2</v>
       </c>
       <c r="G19" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -10869,16 +10809,16 @@
         <v>-0.1224972517047008</v>
       </c>
       <c r="D20" s="3">
-        <v>-1.5063544914680409E-2</v>
+        <v>-1.5456796007699071E-2</v>
       </c>
       <c r="E20" s="3">
-        <v>-8.3669348207884131E-2</v>
+        <v>-8.4965966855257272E-2</v>
       </c>
       <c r="F20" s="3">
         <v>9.6375169573790428E-3</v>
       </c>
       <c r="G20" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -10889,16 +10829,16 @@
         <v>1.170616113744076</v>
       </c>
       <c r="D21" s="3">
-        <v>1.698672114402451</v>
+        <v>1.72</v>
       </c>
       <c r="E21" s="3">
-        <v>1.336349121873337</v>
+        <v>1.343783783783784</v>
       </c>
       <c r="F21" s="3">
         <v>0.92540620384047267</v>
       </c>
       <c r="G21" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -10909,16 +10849,16 @@
         <v>0.16888374783111629</v>
       </c>
       <c r="D22" s="3">
-        <v>0.37582681900180398</v>
+        <v>0.38249694002447981</v>
       </c>
       <c r="E22" s="3">
-        <v>0.16487455197132619</v>
+        <v>0.16653258246178601</v>
       </c>
       <c r="F22" s="3">
         <v>4.5490822027134878E-2</v>
       </c>
       <c r="G22" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -10938,7 +10878,7 @@
         <v>3.6235803136830717E-2</v>
       </c>
       <c r="G23" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -10958,7 +10898,7 @@
         <v>3.0827474310438079E-2</v>
       </c>
       <c r="G24" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -10978,7 +10918,7 @@
         <v>2.4327784891165171E-2</v>
       </c>
       <c r="G25" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -10989,51 +10929,51 @@
         <v>0.19769803656059581</v>
       </c>
       <c r="D26" s="3">
-        <v>0.63840653728294183</v>
+        <v>0.65789473684210531</v>
       </c>
       <c r="E26" s="3">
-        <v>0.22032996274614161</v>
+        <v>0.2237837837837838</v>
       </c>
       <c r="F26" s="3">
         <v>4.2097488921713437E-2</v>
       </c>
       <c r="G26" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -11044,16 +10984,16 @@
         <v>0.96472893533638149</v>
       </c>
       <c r="D31" s="3">
-        <v>0.41500635862653668</v>
+        <v>0.40271301398897841</v>
       </c>
       <c r="E31" s="3">
-        <v>0.52981813055124771</v>
+        <v>0.52164105456083465</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G31" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -11064,16 +11004,16 @@
         <v>373.16181448882872</v>
       </c>
       <c r="D32" s="2">
-        <v>867.45658835546476</v>
+        <v>893.93684210526305</v>
       </c>
       <c r="E32" s="2">
-        <v>679.47844598190522</v>
+        <v>690.12972972972966</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G32" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -11084,16 +11024,16 @@
         <v>7.0151843817787416</v>
       </c>
       <c r="D33" s="3">
-        <v>5.0562770562770556</v>
+        <v>4.9307359307359304</v>
       </c>
       <c r="E33" s="3">
-        <v>10.5852417302799</v>
+        <v>10.43765903307888</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G33" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -11104,16 +11044,16 @@
         <v>51.317254174397043</v>
       </c>
       <c r="D34" s="2">
-        <v>71.198630136986296</v>
+        <v>73.011413520632132</v>
       </c>
       <c r="E34" s="2">
-        <v>34.00961538461538</v>
+        <v>34.490492442710867</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G34" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -11124,16 +11064,16 @@
         <v>0.53738402765144622</v>
       </c>
       <c r="D35" s="3">
-        <v>0.28760282021151579</v>
+        <v>0.27908343125734431</v>
       </c>
       <c r="E35" s="3">
-        <v>0.43809745861506177</v>
+        <v>0.43133597575192351</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G35" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -11144,16 +11084,16 @@
         <v>669.91198375084639</v>
       </c>
       <c r="D36" s="2">
-        <v>1251.7262512768129</v>
+        <v>1289.9368421052629</v>
       </c>
       <c r="E36" s="2">
-        <v>821.73496540713143</v>
+        <v>834.61621621621623</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G36" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -11164,16 +11104,16 @@
         <v>0.48899188876013899</v>
       </c>
       <c r="D37" s="3">
-        <v>0.26592421567295937</v>
+        <v>0.25804699171533341</v>
       </c>
       <c r="E37" s="3">
-        <v>0.41233267500548598</v>
+        <v>0.40596883914856258</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G37" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -11184,54 +11124,54 @@
         <v>736.20853080568725</v>
       </c>
       <c r="D38" s="2">
-        <v>1353.769152196119</v>
+        <v>1395.094736842105</v>
       </c>
       <c r="E38" s="2">
-        <v>873.08142629058011</v>
+        <v>886.76756756756765</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G38" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="G39" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -11251,7 +11191,7 @@
         <v>18.88549618320609</v>
       </c>
       <c r="G44" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -11262,16 +11202,16 @@
         <v>-0.13067027758970889</v>
       </c>
       <c r="D45" s="3">
-        <v>-1.7644637385086821E-2</v>
+        <v>-1.8183263157894741E-2</v>
       </c>
       <c r="E45" s="3">
-        <v>-8.3555082490686536E-2</v>
+        <v>-8.4864864864864858E-2</v>
       </c>
       <c r="F45" s="3">
         <v>5.2483382570162494E-3</v>
       </c>
       <c r="G45" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -11282,16 +11222,16 @@
         <v>0.48899188876013899</v>
       </c>
       <c r="D46" s="3">
-        <v>0.26592421567295937</v>
+        <v>0.25804699171533341</v>
       </c>
       <c r="E46" s="3">
-        <v>0.41233267500548598</v>
+        <v>0.40596883914856258</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G46" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -11308,98 +11248,98 @@
         <v>-1.354047888175353</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G47" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>991</v>
-      </c>
       <c r="G50" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G52" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G53" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G54" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G55" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G56" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G57" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G58" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -11419,7 +11359,7 @@
         <v>3.0827474310438079E-2</v>
       </c>
       <c r="G63" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -11439,27 +11379,27 @@
         <v>2.4327784891165171E-2</v>
       </c>
       <c r="G64" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B66" t="s">
+        <v>985</v>
+      </c>
+      <c r="C66" t="s">
+        <v>986</v>
+      </c>
+      <c r="D66" t="s">
         <v>987</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>988</v>
       </c>
-      <c r="D66" t="s">
+      <c r="F66" t="s">
         <v>989</v>
-      </c>
-      <c r="E66" t="s">
-        <v>990</v>
-      </c>
-      <c r="F66" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -11470,21 +11410,21 @@
         <v>0.19769803656059581</v>
       </c>
       <c r="D67" s="3">
-        <v>0.63840653728294183</v>
+        <v>0.65789473684210531</v>
       </c>
       <c r="E67" s="3">
-        <v>0.22032996274614161</v>
+        <v>0.2237837837837838</v>
       </c>
       <c r="F67" s="3">
         <v>4.2097488921713437E-2</v>
       </c>
       <c r="G67" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -11504,42 +11444,42 @@
         <v>2.3039611964430069E-2</v>
       </c>
       <c r="G69" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G72" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G73" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -11550,16 +11490,16 @@
         <v>1.862085308056872E-3</v>
       </c>
       <c r="D76" s="3">
-        <v>1.7327885597548519E-3</v>
+        <v>1.7856842105263161E-3</v>
       </c>
       <c r="E76" s="3">
-        <v>8.3177221926556679E-4</v>
+        <v>8.4481081081081073E-4</v>
       </c>
       <c r="F76" s="3">
         <v>6.3574593796159528E-4</v>
       </c>
       <c r="G76" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -11579,7 +11519,7 @@
         <v>0.4111810351613478</v>
       </c>
       <c r="G77" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -11591,8 +11531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11605,27 +11545,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>990</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>991</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="B2" s="2">
         <v>121000</v>
@@ -11634,21 +11574,21 @@
         <v>147700</v>
       </c>
       <c r="D2" s="2">
-        <v>97900</v>
+        <v>95000</v>
       </c>
       <c r="E2" s="2">
-        <v>187900</v>
+        <v>185000</v>
       </c>
       <c r="F2" s="2">
         <v>270800</v>
       </c>
       <c r="G2" s="2">
-        <v>165060</v>
+        <v>163900</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B3" s="2">
         <v>152200</v>
@@ -11657,21 +11597,21 @@
         <v>161700</v>
       </c>
       <c r="D3" s="2">
-        <v>116800</v>
+        <v>113900</v>
       </c>
       <c r="E3" s="2">
-        <v>208000</v>
+        <v>205100</v>
       </c>
       <c r="F3" s="2">
         <v>268600</v>
       </c>
       <c r="G3" s="2">
-        <v>181460</v>
+        <v>180300</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B4" s="2">
         <v>214.02</v>
@@ -11694,7 +11634,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B5" s="2">
         <v>17100</v>
@@ -11717,7 +11657,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B6" s="2">
         <v>4257.54</v>
@@ -11740,7 +11680,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B7" s="2">
         <v>8664.1299999999992</v>
@@ -11763,7 +11703,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B8" s="2">
         <v>-61435.69</v>
@@ -11786,30 +11726,30 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B10" s="5">
+        <v>1069</v>
+      </c>
+      <c r="B10" s="4">
         <v>45291</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>44926</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>44561</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>44196</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>43830</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B11" s="3">
         <v>1.257851239669421</v>
@@ -11818,21 +11758,21 @@
         <v>1.09478672985782</v>
       </c>
       <c r="D11" s="3">
-        <v>1.1930541368743619</v>
+        <v>1.198947368421053</v>
       </c>
       <c r="E11" s="3">
-        <v>1.106971793507185</v>
+        <v>1.1086486486486491</v>
       </c>
       <c r="F11" s="3">
         <v>0.99187592319054652</v>
       </c>
       <c r="G11" s="3">
-        <v>1.128907964619867</v>
+        <v>1.1304219819574981</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="B12" s="3">
         <v>0.14132231404958681</v>
@@ -11841,21 +11781,21 @@
         <v>7.9214624238320916E-2</v>
       </c>
       <c r="D12" s="3">
-        <v>8.0922880490296223E-2</v>
+        <v>8.339315789473685E-2</v>
       </c>
       <c r="E12" s="3">
-        <v>5.2694890899414593E-2</v>
+        <v>5.3520918918918921E-2</v>
       </c>
       <c r="F12" s="3">
         <v>5.0221565731166908E-2</v>
       </c>
-      <c r="G12" s="4">
-        <v>8.0875255081757094E-2</v>
+      <c r="G12" s="5">
+        <v>8.1534516166546084E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B13" s="3">
         <v>3.5186280991735527E-2</v>
@@ -11864,21 +11804,21 @@
         <v>2.711726472579553E-2</v>
       </c>
       <c r="D13" s="3">
-        <v>4.0201225740551579E-2</v>
+        <v>4.142842105263158E-2</v>
       </c>
       <c r="E13" s="3">
-        <v>2.1448110697179348E-2</v>
+        <v>2.1784324324324329E-2</v>
       </c>
       <c r="F13" s="3">
         <v>1.723456425406204E-2</v>
       </c>
-      <c r="G13" s="4">
-        <v>2.823748928186481E-2</v>
+      <c r="G13" s="5">
+        <v>2.85501710697098E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B14" s="3">
         <v>7.160438016528925E-2</v>
@@ -11887,21 +11827,21 @@
         <v>5.1223290453622207E-2</v>
       </c>
       <c r="D14" s="3">
-        <v>6.7378855975485194E-2</v>
+        <v>6.9435684210526316E-2</v>
       </c>
       <c r="E14" s="3">
-        <v>3.1411814795103778E-2</v>
+        <v>3.1904216216216218E-2</v>
       </c>
       <c r="F14" s="3">
         <v>3.2807680945347119E-2</v>
       </c>
-      <c r="G14" s="4">
-        <v>5.0885204466969501E-2</v>
+      <c r="G14" s="5">
+        <v>5.1395050398200227E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B15" s="3">
         <v>-0.50773297520661154</v>
@@ -11910,21 +11850,21 @@
         <v>-0.25420399458361542</v>
       </c>
       <c r="D15" s="3">
-        <v>-0.38328988764044952</v>
+        <v>-0.39499031578947369</v>
       </c>
       <c r="E15" s="3">
-        <v>-0.21335838211814789</v>
+        <v>-0.21670291891891891</v>
       </c>
       <c r="F15" s="3">
         <v>-9.2775480059084189E-2</v>
       </c>
-      <c r="G15" s="4">
-        <v>-0.29027214392158168</v>
+      <c r="G15" s="5">
+        <v>-0.29328113691154067</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B16" s="3">
         <v>-2.976190476190476E-7</v>
@@ -11941,7 +11881,7 @@
       <c r="F16" s="3">
         <v>0.4111810351613478</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>